<commit_message>
HRMS DATA ADDED SUCCESSFULLY
</commit_message>
<xml_diff>
--- a/src/main/java/testData/departmentmaster.xlsx
+++ b/src/main/java/testData/departmentmaster.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16095" windowHeight="7170" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16095" windowHeight="7170" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DeptName" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="OrganizationName" sheetId="3" r:id="rId3"/>
     <sheet name="LacationMaster" sheetId="4" r:id="rId4"/>
     <sheet name="BranchMaster" sheetId="5" r:id="rId5"/>
+    <sheet name="LeaveConfiguration" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Description</t>
   </si>
@@ -136,6 +137,21 @@
   </si>
   <si>
     <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Bunit</t>
+  </si>
+  <si>
+    <t>WEEK</t>
+  </si>
+  <si>
+    <t>WeekEND</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
   </si>
 </sst>
 </file>
@@ -685,7 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -722,4 +738,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>